<commit_message>
updated the consensus calculation for multi-label columns, updated some graphs and other small fixes
</commit_message>
<xml_diff>
--- a/gpu outputs/plots/agreement_single_all_400.xlsx
+++ b/gpu outputs/plots/agreement_single_all_400.xlsx
@@ -498,7 +498,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(0.763,0.846)</t>
+          <t>(0.761,0.844)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -1182,7 +1182,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>(0.721,0.81)</t>
+          <t>(0.722,0.811)</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1496,7 +1496,7 @@
         </is>
       </c>
       <c r="D32">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="E32">
         <v>0.46</v>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>(0.6,0.702)</t>
+          <t>(0.601,0.703)</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1542,12 +1542,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>(0.607,0.708)</t>
+          <t>(0.605,0.706)</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>(0.45,0.58)</t>
+          <t>(0.45,0.57)</t>
         </is>
       </c>
     </row>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>(0.535,0.64)</t>
+          <t>(0.533,0.638)</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>(0.628,0.727)</t>
+          <t>(0.629,0.727)</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>(0.544,0.648)</t>
+          <t>(0.545,0.649)</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>(0.65,0.747)</t>
+          <t>(0.651,0.747)</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>(0.616,0.716)</t>
+          <t>(0.617,0.716)</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">

</xml_diff>